<commit_message>
Add line plots for all-caps
</commit_message>
<xml_diff>
--- a/data/MisInfoText/Analysis_output/press_release/MisInfoText_press_release_all_caps.xlsx
+++ b/data/MisInfoText/Analysis_output/press_release/MisInfoText_press_release_all_caps.xlsx
@@ -7,25 +7,24 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="2007" sheetId="1" r:id="rId1"/>
-    <sheet name="2008" sheetId="2" r:id="rId2"/>
-    <sheet name="2009" sheetId="3" r:id="rId3"/>
-    <sheet name="2010" sheetId="4" r:id="rId4"/>
-    <sheet name="2011" sheetId="5" r:id="rId5"/>
-    <sheet name="2012" sheetId="6" r:id="rId6"/>
-    <sheet name="2013" sheetId="7" r:id="rId7"/>
-    <sheet name="2014" sheetId="8" r:id="rId8"/>
-    <sheet name="2016" sheetId="9" r:id="rId9"/>
-    <sheet name="2017" sheetId="10" r:id="rId10"/>
-    <sheet name="2018" sheetId="11" r:id="rId11"/>
-    <sheet name="Proportion Summary" sheetId="12" r:id="rId12"/>
+    <sheet name="2009" sheetId="1" r:id="rId1"/>
+    <sheet name="2010" sheetId="2" r:id="rId2"/>
+    <sheet name="2011" sheetId="3" r:id="rId3"/>
+    <sheet name="2012" sheetId="4" r:id="rId4"/>
+    <sheet name="2013" sheetId="5" r:id="rId5"/>
+    <sheet name="2014" sheetId="6" r:id="rId6"/>
+    <sheet name="2015" sheetId="7" r:id="rId7"/>
+    <sheet name="2016" sheetId="8" r:id="rId8"/>
+    <sheet name="2017" sheetId="9" r:id="rId9"/>
+    <sheet name="2018" sheetId="10" r:id="rId10"/>
+    <sheet name="Proportion Summary" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="245">
   <si>
     <t>factcheckURL</t>
   </si>
@@ -37,59 +36,6 @@
   </si>
   <si>
     <t>proportion_upper_to_alpha_tokens</t>
-  </si>
-  <si>
-    <t>http://www.politifact.com/truth-o-meter/statements/2007/aug/30/john-mccain/mccain-picks-and-chooses-in-attack-on-clinton/</t>
-  </si>
-  <si>
-    <t>"On Monday, Senator Clinton told an audience at the Veterans of Foreign Wars that the surge of troops in Iraq was 'working.' Now, after taking heat from anti-war activists and her primary opponents, Senator Clinton says the surge 'has failed' and that we should 'begin the immediate withdrawal of U.S. troops.'
-"The fact that the New York senator can reverse her position on an issue of grave importance to our national security in a few days sends the wrong signal to our enemies in Iraq and our own troops on the ground.  We must continue to support General Petraeus and the new counterinsurgency campaign to give us the best chance to succeed. Following the path to begin an 'immediate withdrawal' would be a grave mistake."</t>
-  </si>
-  <si>
-    <t>Press release</t>
-  </si>
-  <si>
-    <t>http://www.politifact.com/truth-o-meter/statements/2008/jun/17/republican-national-committee-republican/no-proof-rezko-saved-obama-money-on-home/</t>
-  </si>
-  <si>
-    <t>http://www.politifact.com/truth-o-meter/statements/2009/jan/13/people-american-way/seeing-red-over-warren/</t>
-  </si>
-  <si>
-    <t>A Jury Heard The Facts And Has Judged Obama's Fundraiser Tony Rezko; Shouldn't The American People Be Able To Do The Same?
-AFTER TONY REZKO WAS CONVICTED OF FRAUD YESTERDAY, THERE REMAINS MANY UNANSWERED QUESTIONS ABOUT THE OBAMA REZKO RELATIONSHIP 
-Did Obama Or His Office Do Favors For Tony Rezko?
-"[S]en. Barack Obama's Ties To Indicted Dealmaker Antoin 'Tony' Rezko Include An Internship The Senator Provided The Son Of A Contributor At The Request Of Rezko, An Obama Spokesman Confirmed Saturday." (Frank Main, "Internship Also Links Obama, Rezko," Chicago Sun-Times, 12/24/06)
-Rezko Recommended A Business Associate's Son For "One Of The Coveted Summer Internships" In Obama's Senate Office. "Political fundraiser Antoin 'Tony' Rezko made a modest pitch to U.S. Sen. Barack Obama last year. Rezko recommended a 20-year-old student from Glenview for one of the coveted summer internships in Obama's Capitol Hill office. The student got the job and spent five weeks in Washington, answering Obama's front office phone and logging constituent mail. The student was paid an $804 stipend, about $160 per week, for a position valued mostly for the experience it provides." (David Jackson and Ray Gibson, "Obama Intern Had Ties To Rezko," Chicago Tribune, 12/24/06)
-"As A State Senator, Barack Obama Wrote Letters To City And State Officials Supporting His Political Patron Tony Rezko's Successful Bid To Get More Than $14 Million From Taxpayers To Build Apartments For Senior Citizens." (Tim Novak, "Obama's Letters For Rezko," Chicago Sun-Times, 6/13/07)
-Did Obama Know That Tony Rezko Was Saving Him $300,000 On The Purchase Of His Home?
-Obama Purchased His Chicago Home For $300,000 Less Than The Asking Price While Rezko's Wife, Rita Rezko, Purchased The Adjoining Lot For The Full Asking Price. "Two years ago, Obama bought a mansion on the South Side, in the Kenwood neighborhood, from a doctor. On the same day, Rezko's wife, Rita Rezko, bought the vacant lot next door from the same seller. The doctor had listed the properties for sale together. He sold the house to Obama for $300,000 below the asking price. The doctor got his asking price on the lot from Rezko's wife." (Tim Novak, "Obama And His Rezko Ties," Chicago Sun-Times, 4/23/07)
-Could Obama Have Afforded His Home Without Rezko's Help?
-Obama Originally Said That He Could Not Afford To Purchase The Parcel Of Land Rezko's Wife Purchased And That The House Itself Was Already A Stretch. "It was 'already a stretch' to buy the house, Obama said, so the vacant lot was not affordable for his family." (Ray Gibson and David Jackson, "Rezko Owns Vacant Lot Next To Obama's Home," Chicago Tribune, 11/1/06)
-But Obama Later Said That He Did Not Need Help Purchasing "Both Or Either Of The Tracts" Of Land Involved In The Purchase Of His Chicago Home. Reporter: "Did you generally or expressively state a need for help in buying both or either of the tracts?" Obama: "No, I didn't need help." ("Interview With Obama: Still Confident," Time.com, 3/6/08)
-Did Obama Meet Nadhmi Auchi And Give Him A Toast?
-According To Rezko Trial Testimony, Obama Attended A Reception For Nadhmi Auchi At The Home Of Tony Rezko April 3, 2004. "When Iraqi-born billionaire Nadhmi Auchi attended an April 3, 2004 reception for himself at Tony Rezko's home White House hopeful Barack Obama, and his wife, attended the reception, Stuart Levine testified just now in the trial." (Natasha Korecki, "Obama Bomb Dropped," Chicago Sun-Times' "Eye On Rezko" Blog, http://blogs.suntimes.com/rezko/, 4/14/08)
-"But According To Two Sources Familiar With The Gathering, The Obamas Attended The Wilmette Reception, Which Came Less Than A Month After Obama's Democratic Primary Win For His U.S. Senate Seat." (Natasha Korecki, Chris Fusco and Tim Novak, "Obama's Name In Rezko Trial," Chicago Sun-Times, 4/15/08)
-A Source Told The Chicago Sun-Times That "Obama Not Only Gave Rezko's Guest Of Honor, Iraqi Billionaire Nadhmi Auchi, A Big Welcome . . . But He Made A Few Toasts!" "Dem presidential contender Barack Obama's handlers may be telling the press Obama has NO 'recollection' of a 2004 party at influence peddler Tony Rezko's Wilmette house, but a top Sneed source claims Obama not only gave Rezko's guest of honor, Iraqi billionaire Nadhmi Auchi, a big welcome . . . but he made a few toasts!" (Michael Sneed, "Which Is It? Obamarama..." Chicago Sun-Times, 4/16/08)
-Did Obama Or His Staff Write A Letter To The State Department On Auchi's Behalf?
-Rezko "Asked Certain Illinois Government Officials" To Help Auchi Obtain A Visa To Visit The U.S. After He Had Previously Been Turned Down By The State Department.  "The filing says when Auchi was unable to obtain a visa to visit the United States in 2005, Rezko intervened and 'asked certain Illinois government officials' to appeal the State Department's ruling."  (Brain Ross, "Obama 'Backer' Rezko Ordered To Jail," ABC News' "The Blotter" Blog, www.abcnews.com, 1/28/08)
-The Government Officials Approached Are Not Known, But Sen. Obama Had Just Taken Office In The U.S. Senate In 2005.  "The officials who Rezko approached are not specified. Sen. Obama had just taken office as a U.S. senator in 2005, the same year he sought Rezko's help in the purchase of his home."  (Brain Ross, "Obama 'Backer' Rezko Ordered To Jail," ABC News' "The Blotter" Blog, www.abcnews.com, 1/28/08)
-Has Obama Removed All Rezko Related Funds From His Campaign Coffers As New Rezko Related Donors Have Come To Light?
-Obama Has Acknowledged That Rezko Has Raised About $250,000 For His Campaigns. "For the first time, Sen. Barack Obama put a figure Friday to the amount of campaign contributions that indicted political fund-raiser Tony Rezko raised for the senator's campaigns, and the number -- about $250,000 -- was far more than he previously acknowledged." (Tim Novak, Chris Fusco, Dave McKinney and Carol Marin, "More Rezko Dough Found," Chicago Sun-Times, 3/15/08)
-However The Most Recently Reported Total Of Rezko Related Funds The Obama Campaign Has Donated To Charity Is $160,000. "Obama, seeking to distance himself from his patron [Rezko], has donated $160,000 in Rezko-related contributions to charity." (Dan Morain, "Obama To Be In Background Of Trial," Los Angeles Times, 3/3/08)
-Mustafa Abdalla And Ferras Elshair Posted Properties To Secure Tony Rezko's Release From Jail. "Tony Rezko's $8.5 million bail is being secured by properties and cash linked to friends and family. Here are many of those people and what they'd forfeit if Rezko flees: - Former Iraqi Electricity Minister Aiham Alsammarae and his wife, Amura: an Oak Brook mansion and two South Loop condominiums - Illinois Department of Central Management Services employee Mustafa Abdalla: house in Libertyville - ...  - Former Illinois Department of Central Management Services employee Ferras Elshair: house in Darien..." (Natasha Korecki, Tim Novak and Chris Fusco, "Springing Rezko," Chicago Sun-Times, 4/27/08)
-Mustafa Abdalla, Illinois Department Of Central Management Services Employee, Donated $1,000 To Obama June 30, 2003. (Center For Responsive Politics Website, www.openscrets.org, Accessed 4/29/08)
-Ferras Elshair, Former Illinois Department Of Central Management Services Employee, Donated $250 To Obama May 28, 2004. (Center For Responsive Politics Website, www.openscrets.org, Accessed 4/29/08)
-Semir Sirazi, Who Testified In The Last Week Of Rezko Trial Testimony, Is A 10 Year Friend Of Tony Rezko. "Tony Rezko's 10-year friend, Semir Sirazi, said two checks from Rezko in 2003 -- for $48,000 and $66,000 -- bounced. Sirazi provided consulting services for Rezko's Rezmar companies." (Natasha Korecki, "Witness: Rezko's Checks Bounced," Chicago Sun-Times' "Eye On Rezko" Blog, blogs.suntimes.com, 5/1/08)
-Semir Sirazi Has Donated $4,000 To Barack Obama; $2,000 On 6/30/03 And $2,000 On 6/30/04. (Center For Responsive Politics Website, www.opensecrets.org, Accessed 5/1/08) 
-PDF Format
-A Product Of The RNC Research Department</t>
-  </si>
-  <si>
-    <t>eople For the American Way President Kathryn Kolbert responded today to the news that Rev. Rick Warren of Saddleback Church will deliver the invocation at the presidential inauguration of Barack Obama:
-It is a grave disappointment to learn that pastor Rick Warren will give the invocation at the inauguration of Barack Obama.
-Pastor Warren, while enjoying a reputation as a moderate based on his affable personality and his church's engagement on issues like AIDS in Africa, has said that the real difference between James Dobson and himself is one of tone rather than substance. He has recently compared marriage by loving and committed same-sex couples to incest and pedophilia. He has repeated the Religious Right's big lie that supporters of equality for gay Americans are out to silence pastors. He has called Christians who advance a social gospel Marxists. He is adamantly opposed to women having a legal right to choose an abortion.
-I'm sure that Warren's supporters will portray his selection as an appeal to unity by a president who is committed to reaching across traditional divides. Others may explain it as a response to Warren inviting then-Senator Obama to speak on AIDS and candidate Obama to appear at a forum, both at his church. But the sad truth is that this decision further elevates someone who has in recent weeks actively promoted legalized discrimination and denigrated the lives and relationships of millions of Americans.
-Rick Warren gets plenty of attention through his books and media appearances. He doesn't need or deserve this position of honor. There is no shortage of religious leaders who reflect the values on which President-elect Obama campaigned and who are working to advance the common good.</t>
   </si>
   <si>
     <t>http://www.politifact.com/truth-o-meter/statements/2009/apr/01/michele-bachmann/defending-dollar-bachmann-distorts-geithners-comme/</t>
@@ -150,6 +96,9 @@
   </si>
   <si>
     <t>ObamaCare and gun control Senate Finance Committee Chairman Max Baucus has something to say to gun owners: Own a gun; lose your coverage!Baucus socialized health care bill comes up for a Finance Committee vote on Tuesday. We have waited and waited and waited for the shifty Baucus to release legislative language. But he has refused to release anything but a summary -- and we will never have a Congressional Budget Office cost assessment based on actual legislation. Even the summary was kept secret for a long time.But, on the basis of the summary, the Baucus bill (which is still unnumbered) tells us virtually nothing about what kind of policy Americans will be required to purchase under penalty of law -- nor the consequences. It simply says:* all U.S. citizens and legal residents would be required to purchase coverage through (1) the individual market...;* individuals would be required to report on their federal income tax return the months for which they maintain the required minimum health coverage...;* in addition to an extensive list of statutorily mandated coverage, HHS Secretary Kathleen Sebelius would be empowered to define and update the categories of treatments, items, and services... within an insurance plan which would be covered in a policy constituting required minimum health coverage.It is nearly certain that coverage prescribed by the administration will, to control costs, exclude coverage for what it regards as excessively dangerous activities. And, given Sebelius well-established antipathy to the Second Amendment -- she vetoed concealed carry legislation as governor of Kansas -- we presume she will define these dangerous activities to include hunting and self-defense using a firearm. It is even possible that the Obama-prescribed policy could preclude reimbursement of any kind in a household which keeps a loaded firearm for self-defense.The ObamaCare bill already contains language that will punish Americans who engage in unhealthy behavior by allowing insurers to charge them higher insurance premiums. (What constitutes an unhealthy lifestyle is, of course, to be defined by legislators.) Dont be surprised if an anti-gun nut like Sebelius uses this line of thinking to impose ObamaCare policies which result in a back-door gun ban on any American who owns dangerous firearms.After all, insurers already (and routinely) drop homeowners from their policies for owning certain types of guns or for refusing to use trigger locks (that is, for keeping their guns ready for self-defense!). While not all insurers practice this anti-gun behavior, Gun Owners of America has documented that some do -- Prudential and State Farm being two of the most well-known.The good news is that because homeowner insurance is private (and is still subject to the free market) you can go to another company if one drops you. But what are you going to do under nationalized ObamaCare when the regulations written by Secretary Sebelius suspend the applicability of your government-mandated policy because of your gunownership of this is in addition to something that GOA has been warning you about for several months  the certainty that minimum acceptable policies will dump your gun information into a federal database  a certainty that is reinforced by language in the summary providing for a study to encourage increased meaningful use of electronic health records.Remember, the federal government has already denied more than 150,000 military veterans the right to own guns, without their being convicted of a crime or receiving any due process of law. They were denied because of medical information (such as PTSD) that the FBI later determined disqualified these veterans to own guns.Is this what we need on a national level being applied to every gun owner inAmerica, failure to comply would subject the average family to $1,500 in fines -- and possibly more for a household with older teens. And, although a Schumer amendment purports to exempt Americans from prison sentences for non-purchase of an ObamaPolicy -- something which was never at issue -- it doesnt prohibit them from being sent to prison for a year and fined an additional $25,000 under the Internal Revenue Code for non-payment of the initial fines.Contact your two U.S. Senators. Ask him or her, in the strongest terms, to vote against the phony Baucus bill.You can use the Gun Owners Legislative Action Center to send your senators the pre-written e-mail message below.Dear Senator:You already know that the phony Baucus bill:* Is predicated on $283 billion in phony cuts which have never, never ever been realized since a similar commitment to cut Medicare costs in the Balanced Budget Act of 1997 -- and will never, never ever be realized under the Baucus bill;* Requires massive numbers of Americans to have government-approved insurance which the CBO predicts will be more expensive than current policies;* Refuses to provide a cost for these policies, making it almost certain that more and more Americans will find insurance beyond their reach;* Has no legislative language and nothing but a CBO guesstimate of the cost and benefits, based on a summary.On the basis of the summary, the Baucus bill tells us virtually nothing about what kind of policy Americans will be required to purchase under penalty of law -- nor the consequences. It does say that the Secretary of HHS [Kathleen Sebelius] would be required to define and update the categories of treatments, items, and services... within an insurance plan which would be covered in a policy constituting required minimum health coverage.This could spell trouble for gun owners.It is nearly certain that coverage prescribed by the administration will, to control costs, exclude coverage for what it regards as excessively dangerous activities. And, given Sebelius well-established antipathy to the Second Amendment -- she vetoed concealed carry legislation as governor of Kansas -- I presume she will define these dangerous activities to include hunting and self-defense using a firearm. It is even possible that the Obama-prescribed policy could preclude reimbursement of any kind in a household which keeps a loaded firearm for self-defense.This is, of course, in addition to the certainty that minimum acceptable policies will dump my gun information into a federal database -- a certainty that is reinforced by language in the summary providing for a study to encourage increased meaningful use of electronic health records.Incidentally, failure to comply would subject the average family to $1,500 in fines -- and possibly more for a household with older teens. And, although a Schumer amendment purports to exempt Americans from prison sentences for non-purchase of an ObamaPolicy -- something which was never at issue -- it doesnt prohibit them from being sent to prison for a year and fined an additional $25,000 under the Internal Revenue Code for non-payment of the initial fines.Please oppose the Baucus bill.Sincerely,</t>
+  </si>
+  <si>
+    <t>Press release</t>
   </si>
   <si>
     <t>http://www.politifact.com/georgia/statements/2010/jun/13/kevin-levitas/state-rep-says-georgia-sets-gold-standard-food-saf/</t>
@@ -898,6 +847,98 @@
 Our economic rankings have improved and unemployment has dropped each year, which is a stark contrast to Mary Burke’s policies of higher taxes and large deficits that caused Wisconsin’s rankings to plummet and unemployment to rise above the national average
 During the Doyle-Burke Administration unemployment peaked at 9.2%; under Governor Walker our unemployment rate is at its lowest in 5 years and is now 5.8%
 We can’t afford to go back to policies that bring higher taxes, higher unemployment and job loss. Let’s continue moving forward under Governor Walker’s record of lower unemployment and job creation.</t>
+  </si>
+  <si>
+    <t>https://www.politifact.com/factchecks/2015/oct/13/lynn-westmoreland/Westmoreland-ran-doesnt-have-to-prove-nuclear-plan/</t>
+  </si>
+  <si>
+    <t>https://www.politifact.com/factchecks/2015/oct/28/constitutional-rights-pac/paul-ryan-one-few-gop-vote-force-christian-employe/</t>
+  </si>
+  <si>
+    <t>https://www.politifact.com/factchecks/2015/may/03/robert-hurt/hurt-amiss-linking-estate-tax-small-farm-businesse/</t>
+  </si>
+  <si>
+    <t>https://www.politifact.com/factchecks/2015/jan/23/john-cornyn/cornyn-says-keystone-pipeline-through-texas-create/</t>
+  </si>
+  <si>
+    <t>https://www.politifact.com/factchecks/2015/jan/18/bobby-scott/bobby-scott-low-gas-prices-are-result-obama-polici/</t>
+  </si>
+  <si>
+    <t>https://www.politifact.com/factchecks/2015/apr/13/dave-brat/brat-says-obamacare-repeal-would-save-nation-2-tri/</t>
+  </si>
+  <si>
+    <t>https://www.politifact.com/factchecks/2015/mar/10/state-democratic-party-wisconsin/democratic-party-says-scott-walker-proposed-sellin/</t>
+  </si>
+  <si>
+    <t>WASHINGTON, D.C. – Today, Representative Lynn Westmoreland issued the following statement after he voted ‘no’ on H.R. 3461, a bill to approve the Joint Comprehensive Plan of Action, signed at Vienna on July 14, 2015, relating to the nuclear program of Iran:
+“We do not need to be negotiating with Iran - period. Iran is a dangerous nation that cannot be trusted and this deal only weakens the national security of our country and that of our allies – particularly Israel. Like many times before, President Obama is manipulating the system to get his way: presenting this to the American people as a ‘deal’ instead of what it really is –a treaty – to circumvent needing approval by Congress. President Obama and Secretary Kerry also showed a lack of leadership and strength in agreeing to lift Iran’s economic and arms sanctions without any proof of change in conduct. The administration put the ball in Iran’s hands, and it will forever be a huge mistake.
+“I came to Congress to make our country and our world a safer and better place for my children and grandchildren, and this deal does not do either. Not only do I reject this agreement, but I reject the President’s secretive manipulation and the negotiations with Iran entirely.”
+In addition to voting NO on H.R. 3461, the approval of the Joint Comprehensive Plan of Action, Rep. Westmoreland voted in support of H.R. 3460, which would prevent the President from ending the current sanctions against Iran.
+For more information about our releases, please contact 202-225-5901.</t>
+  </si>
+  <si>
+    <t>Washington, DC – The coalition of conservatives and conservative organizations that recently forced Rep. Kevin McCarthy to forsake his pursuit of the the top post in the United States House today launched a campaign opposing Rep. Paul Ryan.
+"Paul Ryan is undeserving of the Speakership," says Fire Paul Ryan organizer and Chairman of Constitutional Rights PAC Larry Ward  "We fought Rep. McCarthy's race to lead the House because of his compromises, and we aren't going to turn a blind eye toward's Ryan, despite the fact that he presents himself as a conservative."
+The coalition's website, FirePaulRyan.com, urges Americans to pledge to "Fire Paul Ryan" should he become the Speaker of the House of Representatives, and, like the Fire McCarthy project, focuses on Ryan's poor reception among conservatives.
+“Just like John Boehner and his deputy Kevin McCarthy, Paul Ryan scores terribly with conservatives,” says FirePaulRyan.com, adding:
+• Heritage Action scores Ryan at an awful 55
+• Conservative Review assigned him an F-rating at 58
+• The New American's Freedom Index also scores him at a low 58 
+Coalition member and former U.S. Congressman Paul Broun (R-Ga.) believes that Paul Ryan will continue the failed policies of John Boehner to the detriment of the American people.  
+"I like Paul Ryan personally, but I believe that if he were to be elected Speaker we will see a continuation of Boehner policies," Broun says. "We must elect a Speaker that will stand-up to Obama and his radical policies that are hurting all Americans, especially the poor and senior citizens on limited incomes. We have to have leadership that is strong and truly conservative."
+Like Broun, former U.S. Senate candidate Col. Rob Maness (Ret) argues that this country "needs a speaker of the house that will support a strategy based on conservative principles and winning ideas – not a speaker that will support party principles and losing ideas.”
+After personally taking the pledge to Fire Paul Ryan, conservative candidate for Congress Kay Daly is now challenging her opponent, Rep. Renee Ellmers (RINO-NC2), to join the coalition and oppose Ryan as Speaker.
+“Paul Ryan would be the most liberal, pro-union, Republican Speaker in history," says Daly. "He is one of only six House Republicans who voted for Teddy Kennedy’s bill to force Christian employers to hire LGBT employees. Even John Boehner never did that!”
+Alan Keyes of Americans United for Freedom says Rep. Boehner’s resignation "creates major opportunity to select an individual committed to restoring the American Republic" – he too is a signatory of the Fire Paul Ryan pledge. 
+Ken Benway, LTC, USA (Ret.), Special Operations Speaks co-founder said "The veteran community has not forgotten the Ryan-Murray budget which targeted massive cuts to military retirement. We can not back a speaker that turned his back on the veteran community." 
+The Fire Paul Ryan coalition exists to demand a conservative be selected to lead a "bottom-up" United States House of Representatives.
+"We forced Boehner to step down, Cantor was defeated, and McCarthy withdrew – yet the Establishment continues to serve up RINO after RINO after RINO," says Ward. "If Ryan is chosen, we’ll see that he’s fired."
+Constitutional Rights PAC's campaign to Fire Paul Ryan is supported by prominent conservatives including former U.S. Congressman Paul Broun, Alan Keyes, Larry Klayman, and Col. Rob Maness (Ret), Larry Ward and a growing number of organizations including American Dream Initiative, Conservative Action Fund, FreedomWatch, GatorPAC, Life &amp; Liberty PAC, Madison Project, PatriotPAC, Political Media, Special Operations Speaks PAC, and 1776 Coalition.
+For more details visit FirePaulRyan.com.
+###</t>
+  </si>
+  <si>
+    <t>WASHINGTON, D.C. – Congressman Robert Hurt (R-Virginia) released the following statement after voting in favor of the Death Tax Repeal Act, which would repeal the estate and generation transfer skipping tax and reduce the highest gift tax rate:
+“The death tax causes serious problems for family farmers and small business owners who want to have their children and grandchildren continue their life’s work. In many cases, this excessive and duplicative tax forces them to sell the farm or business just to pay these punitive taxes, keeping them from passing down the culmination of their lifetime of work to the next generation. Our vote to repeal the death tax today is a crucial step toward implementing a simpler, fairer tax code and ensuring that our small businesses can continue to create the jobs Virginia’s Fifth District needs.
+“We must continue to free our Main Street businesses and family farms from government-created obstacles to economic growth, and I remain committed to advancing policies that will spur job creation and economic recovery. I was proud to cosponsor this commonsense legislation and see it pass the House with bipartisan support. I urge our colleagues in the Senate to continue working with us to promote success for our small businesses and family farms so that they can create jobs and generate opportunity and prosperity for our communities.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Tuesday marked the start of the 114th Congress, with fresh leadership and a new commitment to the American people.  We’re working to restore the Senate to its original purpose: a forum where we can discuss, debate, and pass legislation to benefit citizens.  That’s why we’re beginning with bipartisan legislation, like the approval of the Keystone XL Pipeline.  But the President has already threatened to veto this economy-boosting bill and prevent it from becoming law.
+It’s unfortunate that the President would shut down this bipartisan legislation.  In Texas, we’ve seen the direct positive impact of the pipeline on the local and state economy.  The Texas leg of the project, which delivers more than 400,000 barrels of crude oil from Cushing, OK to Southeast Texas each day, has already created 4,800 jobs in just the year it's been up and running. 
+I promise to keep fighting for pro-growth legislation like this to get America back on track.  In fact, I’ve already introduced a bill to provide a permanent deduction for state and local sales taxes on your federal tax returns, which will allow you keep more of your hard-earned money in your pocket.  I also re-introduced legislation to crack down on human traffickers and lend their victims a helping hand to end these terrible crimes.
+As the year goes on, I’ll continue to look for areas where we can promote economic growth and strong Texas values across America. </t>
+  </si>
+  <si>
+    <t>WASHINGTON, D.C. – Congressman Robert C. “Bobby” Scott (VA-03) issued the following statement on his vote against H.R. 3, the latest attempt by House Republicans to force an approval of the Keystone XL Pipeline:
+“Supporters of the Keystone XL Pipeline believe that construction of the pipeline will create jobs and move our nation closer to energy independence by reducing our reliance on foreign oil. However, these beliefs fail to recognize the current economic climate.  Last year, the United States produced more oil domestically than was imported, and gas prices are, and are expected to remain, near lows not seen in years.  Even if this were not the case, much of the tar sands oil that would run through this new pipeline would not be sold in the United States and would have no effect on domestic gas prices, but would instead pass through our nation for eventual sale on international markets. 
+“Additionally, the long term economic benefits of this pipeline do not justify risking our nation's drinking water, farmlands, and tribal grounds.  Cleanup costs from a 2010 tar sands oil pipeline spill in Kalamazoo, Michigan have exceeded $1 billion. To add insult to injury, companies that produce, ship, or refine tar sands oil are not required to pay into the Oil Spill Liability Trust Fund, which conventional crude oil companies pay into,  and therefore the cost of cleaning up tar sands oil spills will fall on the American taxpayer.
+"According to the State Department's Final Environmental Impact Statement, the project would only directly create 2,000 temporary jobs and few as 35 permanent jobs.  Last month, our economy grew by more than 250,000 jobs and is currently creating more jobs in two hours of an average work day than the temporary jobs that would be created by this project, and more jobs in one and a half average workday minutes than the permanent jobs created. 
+"Instead of exempting foreign corporations from federal permitting requirements, Congress should be working on policies that diversify our nation’s energy portfolio, reduce our reliance on fossil fuels, and support the President’s policies that have resulted in gas prices being reduced from $3.07 per gallon when he was sworn in in 2009 to $2.30 today.”
+# # #</t>
+  </si>
+  <si>
+    <t>Washington, DC (March 17, 2015) – Statement from Rep. Dave Brat (R-VA), a member of the House Budget Committee, on the House budget released today:
+“Today, Republicans are presenting a budget that will balance the federal budget in less than 10 years through reductions in duplicative and wasteful spending; a budget that will fully repeal Obamacare and allow for alternatives that actually lower costs; and a budget that will reform entitlement programs to support those in need, prevent fraud, and ensure these programs are financially sustainable so they are available for future generations.
+“House Republicans have released a budget that will take aim at fixing some of the greatest threats currently facing our nation.
+“The first priority of this budget proposal is to balance the federal budget in less than 10 years by making $5.5 trillion in spending reductions over the course of that time. Under current policy, the federal government will spend $48.6 trillion over the next 10 years. Under this proposal, it will spend roughly $43.2 trillion.  This budget responsibly reforms government spending while avoiding heavy-handed cuts – protecting key priorities while eliminating waste and modernizing programs. As former chairman of the Joint Chiefs of Staff Admiral Mike Mullen has said, our debt is ‘the single, biggest threat to our national security.’  This budget aims to tackle this threat head-on, because we cannot achieve national security without economic security. 
+“This budget fulfills Republicans’ pledge to voters to repeal Obamacare in its entirety – including all of the tax increases, job-killing regulations, and mandates – saving our nation more than $2 trillion.  Instead of a complex structure of subsidies, mandates, and penalties, this budget increases access to affordable health care by expanding choices and flexibility for individuals, families, and businesses.  For instance, this budget will empower states -- not Washington -- to tailor their Medicaid programs so that they can best serve the most vulnerable of their citizens. The budget also proposes to reform Medicare to harness the power of consumer choice that has made the prescription drug plan under Medicare Part D so popular. 
+“This budget will ensure better care for our veterans by working to enhance oversight over the Department of Veterans Affairs and its bureaucratic mismanagement. We will continue working to ensure that we provide sufficient resources to our veterans to more effectively provide benefits to those who have fought to defend our country and our way of life.
+“This budget builds upon the work of the House Education and the Workforce Committee to consolidate federal job-training programs, which will produce better results for the millions of Americans looking to improve their skills in their search for jobs.
+“This budget will provide some desperately needed reforms to entitlement programs.  Federal spending for food stamps, the Supplemental Nutrition Assistance Program (SNAP), has increased from $21 billion in 2002 to $76 billion in 2014. Our budget calls for reduced funding for federal advertising efforts to increase SNAP enrollment. Those savings are then shifted into programs that help people get off permanent dependency, such as job-training programs.
+“This budget recommends easing the burden of regulations on American workers and their employers. It calls on Congress to enact legislation to reform our regulatory system by eliminating unnecessary red tape and by ensuring that regulations do not disproportionately disadvantage low-income Americans.  Since President Obama took office in January 2009, the federal government has issued more than 468,500 pages of regulations. The overwhelming amount and burdensome nature of these regulations are hurting our economy. The National Association of Manufacturers estimates the total cost of regulations is as high as $2.03 trillion per year, and compliance costs fall ‘disproportionately on small businesses.’ This translates into fewer job opportunities for American workers and much higher costs for consumers.
+“This budget also seeks to eliminate several corporate welfare programs, reaffirming our commitment to stopping cronyism. This budget makes clear that Washington should not be in the business of picking the winners and losers of our economy in the private sector.  The best way to ensure a vibrant and strong economy is to allow innovators to thrive based on merit and the actual consumer demand for their products and services -- not based on the powerful friends they have in Washington. 
+“Today, six years into our very weak recovery, wages are stagnant, median income is down, debt has mounted on the backs of children not yet born, and economic growth is sputtering. Hard-working American families are struggling as average hourly wages are barely keeping pace with inflation, real median household income is just under $52,000 – one of the lowest levels since the mid-1990s – and an unhealthy percentage of the American workforce has dropped out of the labor market. 
+“Between the thousands of pages of ineffective and overburdening regulations, the millions of unemployed American workers, and the trillions in out-of-control spending, it is clear that we have trillion dollar problems that call for trillion dollar solutions.  This budget – with its serious and common sense proposals – represents a solid first step toward reining in uncontrolled federal spending, turning our economy around, and creating an environment that spurs job creation and higher wages for all Americans.”
+The proposed fiscal year 2016 House budget is here.</t>
+  </si>
+  <si>
+    <t>Lost amid the contentious Right to Work legislation being fast-tracked through the legislature this week as Scott Walker campaigns for president around the country are Joint Finance Committee hearings on Walker's "Iowa Caucus Budget," but the sweeping changes Walker has proposed to the state Department of Natural Resources are starting to get the attention they deserve as even Republican legislators are questioning the plans, which include a proposal to sell naming rights to our state parks.
+Scott Walker might not live here anymore as he campaigns for president around the country, merely "visiting" Wisconsin from time to time, but millions of Wisconsinites value our conservation heritage and the preservation of our state park system -- so Walker's Iowa Caucus Budget proposal that guts funding for state parks is already cause for alarm. In addition to the fee increases proposed in Walker's budget, DNR Secretary Cathy Stepp yesterday told members of the Joint Finance Committee that the state was looking at several other options to generate revenue, like selling naming rights to our natural resources to offset Walker's cuts. 
+Exclusive access for corporate donors to Wisconsin's farm and forest land and valuable state real estate has been a hallmark of Scott Walker's time in office. Scott Walker proposed in his 2013 budget changes to state law to allow foreign companies and individuals to buy large tracts of land, like farms, that are over 640 acres in size. Republicans and Democrats alike voiced concerns, and the proposal was deleted by the Joint Finance Committee. The Wisconsin Farm Bureau Federation also opposed the changes. On his way out of office to a cushy lobbying job in Washington, D.C., Attorney General J.B. Van Hollen greenlit the Walker land proposal.
+Another provision of the 2013 budget allowed the Walker administration to sell off state assets without a competitive bidding process. Included for sale are telecommunications towers and related infrastructure around the state, administrative buildings in Madison and Milwaukee, the Northern Wisconsin Center in Chippewa Falls, and land surrounding the state Department of Transportation building that has been described as prime commercial real estate.
+Also in 2013 a group calling itself United Sportsmen of Wisconsin, a Tea Party group funded by the Koch brothers and headed by a Walker political insider, was almost the recipient of a $500,000 grant inserted by then-Rep. Scott Suder into the state budget for the purpose of promoting hunting, fishing and trapping in Wisconsin. United Sportsmen was found to have no history of outdoors training; their record more closely mirrored a lobbying organization for Republican interests and several prominent board members were found to have donated to Republican candidates and causes. It was only after United Sportsmen falsified its application to the state and at a hearing before the Joint Finance Committee in stating that they had a federal 501(c)(3) nonprofit designation did the Walker administration finally cancel the grant.
+And following a $700,000 donation to Wisconsin Club for Growth for Scott Walker in exchange for access to the legislative process, the out-of-state mining company Gogebic Taconite was able to draft their own legislation, with assistance from the Governor's Office, on a controversial mining proposal that endangered Wisconsin's natural resources. Just last week, however, the company announced it was no longer going to continue with the project and they would not create the jobs promised.
+"As someone who simply 'visits' Wisconsin as he campaigns for president, Scott Walker might not remember that our state parks are vital to Wisconsin's conservation heritage," Democratic Party of Wisconsin Chair Mike Tate said Wednesday. "Are we going to see Donald Trump Trail or Koch Springs? McRib Mountain? This is absurd. The people who do live here in Wisconsin, and love our state, deserve better than Walker's short-sighted giveaways to corporate special interests that threaten our state's richest assets, our natural resources."</t>
   </si>
   <si>
     <t>http://www.politifact.com/wisconsin/statements/2016/apr/11/chris-larson/chris-larson-says-chris-abele-spent-42-vote-spring/</t>
@@ -1615,7 +1656,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1640,18 +1681,78 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>0.03658536585365853</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>0.03319502074688797</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
-        <v>0.008</v>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>0.01358695652173913</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>0.01123595505617977</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>0.008936550491510277</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1659,7 +1760,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1681,254 +1782,855 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>178</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>229</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D2">
-        <v>0.05741626794258373</v>
+        <v>0.08728179551122195</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>179</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>197</v>
+        <v>230</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>0.05422314911366007</v>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>231</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>0.04659498207885305</v>
+        <v>0.0130718954248366</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>181</v>
+        <v>225</v>
       </c>
       <c r="B5" t="s">
-        <v>199</v>
+        <v>232</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>0.04069767441860465</v>
+        <v>0.009960159362549801</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>182</v>
+        <v>226</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>233</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>0.03271028037383177</v>
+        <v>0.00906344410876133</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>183</v>
+        <v>227</v>
       </c>
       <c r="B7" t="s">
-        <v>201</v>
+        <v>234</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>0.03076923076923077</v>
+        <v>0.007722007722007722</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>184</v>
+        <v>228</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>235</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D8">
-        <v>0.02920443101711984</v>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>0.02070796973399514</v>
+      </c>
+      <c r="D2">
+        <v>0.0131054602432298</v>
+      </c>
+      <c r="E2">
+        <v>0.008936550491510277</v>
+      </c>
+      <c r="F2">
+        <v>0.01123595505617977</v>
+      </c>
+      <c r="G2">
+        <v>0.01358695652173913</v>
+      </c>
+      <c r="H2">
+        <v>0.03319502074688797</v>
+      </c>
+      <c r="I2">
+        <v>0.03658536585365853</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>0.01551575996402847</v>
+      </c>
+      <c r="D3">
+        <v>0.007968797795563106</v>
+      </c>
+      <c r="E3">
+        <v>0.005917159763313609</v>
+      </c>
+      <c r="F3">
+        <v>0.008981574281088582</v>
+      </c>
+      <c r="G3">
+        <v>0.01421911421911422</v>
+      </c>
+      <c r="H3">
+        <v>0.02267693629962646</v>
+      </c>
+      <c r="I3">
+        <v>0.02617801047120419</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>0.01650482276044386</v>
+      </c>
+      <c r="D4">
+        <v>0.01189264657558727</v>
+      </c>
+      <c r="E4">
+        <v>0.002688172043010753</v>
+      </c>
+      <c r="F4">
+        <v>0.00641025641025641</v>
+      </c>
+      <c r="G4">
+        <v>0.01421800947867299</v>
+      </c>
+      <c r="H4">
+        <v>0.02395209580838323</v>
+      </c>
+      <c r="I4">
+        <v>0.03875968992248062</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>0.02133109068316243</v>
+      </c>
+      <c r="D5">
+        <v>0.0160387086298822</v>
+      </c>
+      <c r="E5">
+        <v>0.002906976744186046</v>
+      </c>
+      <c r="F5">
+        <v>0.01115859449192783</v>
+      </c>
+      <c r="G5">
+        <v>0.01751787538304392</v>
+      </c>
+      <c r="H5">
+        <v>0.02689025019788691</v>
+      </c>
+      <c r="I5">
+        <v>0.05604483586869496</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B6">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>0.02050214905726718</v>
+      </c>
+      <c r="D6">
+        <v>0.01665099183681952</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.009950248756218905</v>
+      </c>
+      <c r="G6">
+        <v>0.01526717557251908</v>
+      </c>
+      <c r="H6">
+        <v>0.03091190108191654</v>
+      </c>
+      <c r="I6">
+        <v>0.05990783410138249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>0.02926271851434809</v>
+      </c>
+      <c r="D7">
+        <v>0.02253099872992845</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.01396535625744551</v>
+      </c>
+      <c r="G7">
+        <v>0.02824858757062147</v>
+      </c>
+      <c r="H7">
+        <v>0.03485576923076923</v>
+      </c>
+      <c r="I7">
+        <v>0.08279569892473118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>0.02225783083589672</v>
+      </c>
+      <c r="D8">
+        <v>0.01260499208312347</v>
+      </c>
+      <c r="E8">
+        <v>0.004761904761904762</v>
+      </c>
+      <c r="F8">
+        <v>0.0134164174144234</v>
+      </c>
+      <c r="G8">
+        <v>0.02521008403361345</v>
+      </c>
+      <c r="H8">
+        <v>0.03105737316263632</v>
+      </c>
+      <c r="I8">
+        <v>0.03688524590163934</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>0.08320279318099762</v>
+      </c>
+      <c r="D9">
+        <v>0.211277473790521</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.01339078938662079</v>
+      </c>
+      <c r="G9">
+        <v>0.02043992349156668</v>
+      </c>
+      <c r="H9">
+        <v>0.0413230667329028</v>
+      </c>
+      <c r="I9">
+        <v>0.8105263157894737</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B10">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>0.02681745890813439</v>
+      </c>
+      <c r="D10">
+        <v>0.01557921114080659</v>
+      </c>
+      <c r="E10">
+        <v>0.003891050583657588</v>
+      </c>
+      <c r="F10">
+        <v>0.0154442279032443</v>
+      </c>
+      <c r="G10">
+        <v>0.02732009667610905</v>
+      </c>
+      <c r="H10">
+        <v>0.03222501797268152</v>
+      </c>
+      <c r="I10">
+        <v>0.05741626794258373</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>0.02038918601848249</v>
+      </c>
+      <c r="D11">
+        <v>0.02990004112061117</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.008392725915384525</v>
+      </c>
+      <c r="G11">
+        <v>0.009960159362549801</v>
+      </c>
+      <c r="H11">
+        <v>0.0143484477124183</v>
+      </c>
+      <c r="I11">
+        <v>0.08728179551122195</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>0.02617801047120419</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>0.02366863905325444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>0.0223463687150838</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>0.01818181818181818</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>0.01025641025641026</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>0.009174311926605505</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>0.008403361344537815</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>185</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>203</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D9">
-        <v>0.02836879432624113</v>
+        <v>0.005917159763313609</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>0.03875968992248062</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>0.03560371517027864</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>0.03508771929824561</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>0.02810304449648712</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>0.02395209580838323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>0.01941747572815534</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>0.01822916666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>0.0149812734082397</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>186</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>204</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D10">
-        <v>0.02824267782426778</v>
+        <v>0.01421800947867299</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>187</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>205</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D11">
-        <v>0.02639751552795031</v>
+        <v>0.01183431952662722</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>188</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>206</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D12">
-        <v>0.02185792349726776</v>
+        <v>0.00796812749003984</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>189</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>207</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D13">
-        <v>0.02180685358255452</v>
+        <v>0.007092198581560284</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>190</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D14">
-        <v>0.02153846153846154</v>
+        <v>0.00641025641025641</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>191</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>209</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D15">
-        <v>0.01341281669150522</v>
+        <v>0.006309148264984227</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>192</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>210</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D16">
-        <v>0.01020082881734141</v>
+        <v>0.006006006006006006</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>193</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>211</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D17">
-        <v>0.009036144578313253</v>
+        <v>0.00392156862745098</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>194</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>212</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D18">
-        <v>0.006345177664974619</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B19" t="s">
-        <v>213</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19">
-        <v>0.003891050583657588</v>
+        <v>0.002688172043010753</v>
       </c>
     </row>
   </sheetData>
@@ -1950,15 +2652,14 @@
     <hyperlink ref="A16" r:id="rId15"/>
     <hyperlink ref="A17" r:id="rId16"/>
     <hyperlink ref="A18" r:id="rId17"/>
-    <hyperlink ref="A19" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1980,769 +2681,170 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>214</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D2">
-        <v>0.08728179551122195</v>
+        <v>0.05604483586869496</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>215</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>0.015625</v>
+        <v>0.04117647058823529</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>216</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>0.0130718954248366</v>
+        <v>0.03673469387755102</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>217</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>0.009960159362549801</v>
+        <v>0.02360876897133221</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>218</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>0.00906344410876133</v>
+        <v>0.02277904328018223</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>219</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>226</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>0.007722007722007722</v>
+        <v>0.01818181818181818</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>220</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>227</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1">
-        <v>2007</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0.008</v>
-      </c>
-      <c r="E2">
-        <v>0.008</v>
-      </c>
-      <c r="F2">
-        <v>0.008</v>
-      </c>
-      <c r="G2">
-        <v>0.008</v>
-      </c>
-      <c r="H2">
-        <v>0.008</v>
-      </c>
-      <c r="I2">
-        <v>0.008</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1">
-        <v>2008</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>0.02378463379097123</v>
-      </c>
-      <c r="D3">
-        <v>0.01869767602439819</v>
-      </c>
-      <c r="E3">
-        <v>0.01056338028169014</v>
-      </c>
-      <c r="F3">
-        <v>0.01717400703633068</v>
-      </c>
-      <c r="G3">
-        <v>0.02378463379097123</v>
-      </c>
-      <c r="H3">
-        <v>0.03039526054561177</v>
-      </c>
-      <c r="I3">
-        <v>0.03700588730025231</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1">
-        <v>2009</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>0.02070796973399514</v>
-      </c>
-      <c r="D4">
-        <v>0.0131054602432298</v>
-      </c>
-      <c r="E4">
-        <v>0.008936550491510277</v>
-      </c>
-      <c r="F4">
-        <v>0.01123595505617977</v>
-      </c>
-      <c r="G4">
-        <v>0.01358695652173913</v>
-      </c>
-      <c r="H4">
-        <v>0.03319502074688797</v>
-      </c>
-      <c r="I4">
-        <v>0.03658536585365853</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1">
-        <v>2010</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>0.01551575996402847</v>
-      </c>
-      <c r="D5">
-        <v>0.007968797795563106</v>
-      </c>
-      <c r="E5">
-        <v>0.005917159763313609</v>
-      </c>
-      <c r="F5">
-        <v>0.008981574281088582</v>
-      </c>
-      <c r="G5">
-        <v>0.01421911421911422</v>
-      </c>
-      <c r="H5">
-        <v>0.02267693629962646</v>
-      </c>
-      <c r="I5">
-        <v>0.02617801047120419</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="1">
-        <v>2011</v>
-      </c>
-      <c r="B6">
-        <v>17</v>
-      </c>
-      <c r="C6">
-        <v>0.01650482276044386</v>
-      </c>
-      <c r="D6">
-        <v>0.01189264657558727</v>
-      </c>
-      <c r="E6">
-        <v>0.002688172043010753</v>
-      </c>
-      <c r="F6">
-        <v>0.00641025641025641</v>
-      </c>
-      <c r="G6">
-        <v>0.01421800947867299</v>
-      </c>
-      <c r="H6">
-        <v>0.02395209580838323</v>
-      </c>
-      <c r="I6">
-        <v>0.03875968992248062</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1">
-        <v>2012</v>
-      </c>
-      <c r="B7">
-        <v>12</v>
-      </c>
-      <c r="C7">
-        <v>0.02133109068316243</v>
-      </c>
-      <c r="D7">
-        <v>0.0160387086298822</v>
-      </c>
-      <c r="E7">
-        <v>0.002906976744186046</v>
-      </c>
-      <c r="F7">
-        <v>0.01115859449192783</v>
-      </c>
-      <c r="G7">
-        <v>0.01751787538304392</v>
-      </c>
-      <c r="H7">
-        <v>0.02689025019788691</v>
-      </c>
-      <c r="I7">
-        <v>0.05604483586869496</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="1">
-        <v>2013</v>
-      </c>
-      <c r="B8">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>0.02050214905726718</v>
-      </c>
-      <c r="D8">
-        <v>0.01665099183681952</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0.009950248756218905</v>
-      </c>
-      <c r="G8">
-        <v>0.01526717557251908</v>
-      </c>
-      <c r="H8">
-        <v>0.03091190108191654</v>
-      </c>
-      <c r="I8">
-        <v>0.05990783410138249</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1">
-        <v>2014</v>
-      </c>
-      <c r="B9">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>0.02926271851434809</v>
-      </c>
-      <c r="D9">
-        <v>0.02253099872992845</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0.01396535625744551</v>
-      </c>
-      <c r="G9">
-        <v>0.02824858757062147</v>
-      </c>
-      <c r="H9">
-        <v>0.03485576923076923</v>
-      </c>
-      <c r="I9">
-        <v>0.08279569892473118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="1">
-        <v>2016</v>
-      </c>
-      <c r="B10">
-        <v>14</v>
-      </c>
-      <c r="C10">
-        <v>0.08320279318099762</v>
-      </c>
-      <c r="D10">
-        <v>0.211277473790521</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0.01339078938662079</v>
-      </c>
-      <c r="G10">
-        <v>0.02043992349156668</v>
-      </c>
-      <c r="H10">
-        <v>0.0413230667329028</v>
-      </c>
-      <c r="I10">
-        <v>0.8105263157894737</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1">
-        <v>2017</v>
-      </c>
-      <c r="B11">
-        <v>18</v>
-      </c>
-      <c r="C11">
-        <v>0.02681745890813439</v>
-      </c>
-      <c r="D11">
-        <v>0.01557921114080659</v>
-      </c>
-      <c r="E11">
-        <v>0.003891050583657588</v>
-      </c>
-      <c r="F11">
-        <v>0.0154442279032443</v>
-      </c>
-      <c r="G11">
-        <v>0.02732009667610905</v>
-      </c>
-      <c r="H11">
-        <v>0.03222501797268152</v>
-      </c>
-      <c r="I11">
-        <v>0.05741626794258373</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="1">
-        <v>2018</v>
-      </c>
-      <c r="B12">
-        <v>7</v>
-      </c>
-      <c r="C12">
-        <v>0.02038918601848249</v>
-      </c>
-      <c r="D12">
-        <v>0.02990004112061117</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0.008392725915384525</v>
-      </c>
-      <c r="G12">
-        <v>0.009960159362549801</v>
-      </c>
-      <c r="H12">
-        <v>0.0143484477124183</v>
-      </c>
-      <c r="I12">
-        <v>0.08728179551122195</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>0.03700588730025231</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>0.01056338028169014</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>0.03658536585365853</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>0.03319502074688797</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>0.01358695652173913</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>0.01123595505617977</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>0.008936550491510277</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>0.02617801047120419</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>0.02366863905325444</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>0.0223463687150838</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>0.01818181818181818</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>0.01025641025641026</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>0.009174311926605505</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8">
-        <v>0.008403361344537815</v>
+        <v>0.01685393258426966</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D9">
-        <v>0.005917159763313609</v>
+        <v>0.01304347826086956</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>0.01282051282051282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>0.006172839506172839</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>0.005649717514124294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>0.002906976744186046</v>
       </c>
     </row>
   </sheetData>
@@ -2755,6 +2857,10 @@
     <hyperlink ref="A7" r:id="rId6"/>
     <hyperlink ref="A8" r:id="rId7"/>
     <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A13" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2784,240 +2890,240 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D2">
-        <v>0.03875968992248062</v>
+        <v>0.05990783410138249</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>0.03560371517027864</v>
+        <v>0.04424778761061947</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>0.03508771929824561</v>
+        <v>0.0396039603960396</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>0.02810304449648712</v>
+        <v>0.03703703703703703</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>0.02395209580838323</v>
+        <v>0.03091190108191654</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>0.01941747572815534</v>
+        <v>0.02456140350877193</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D8">
-        <v>0.01822916666666667</v>
+        <v>0.01907356948228883</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D9">
-        <v>0.0149812734082397</v>
+        <v>0.01718213058419244</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D10">
-        <v>0.01421800947867299</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D11">
-        <v>0.01183431952662722</v>
+        <v>0.01456310679611651</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D12">
-        <v>0.00796812749003984</v>
+        <v>0.01232032854209446</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D13">
-        <v>0.007092198581560284</v>
+        <v>0.01043478260869565</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D14">
-        <v>0.00641025641025641</v>
+        <v>0.009950248756218905</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D15">
-        <v>0.006309148264984227</v>
+        <v>0.007194244604316547</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D16">
-        <v>0.006006006006006006</v>
+        <v>0.003703703703703704</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D17">
-        <v>0.00392156862745098</v>
+        <v>0.002577319587628866</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>122</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D18">
-        <v>0.002688172043010753</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3046,7 +3152,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3068,170 +3174,526 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D2">
-        <v>0.05604483586869496</v>
+        <v>0.08279569892473118</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>0.04117647058823529</v>
+        <v>0.04878048780487805</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>0.03673469387755102</v>
+        <v>0.03485576923076923</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>0.02360876897133221</v>
+        <v>0.03485576923076923</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>0.02277904328018223</v>
+        <v>0.02994011976047904</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>0.01818181818181818</v>
+        <v>0.02824858757062147</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D8">
-        <v>0.01685393258426966</v>
+        <v>0.02586206896551724</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>78</v>
+        <v>130</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D9">
-        <v>0.01304347826086956</v>
+        <v>0.01532567049808429</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D10">
-        <v>0.01282051282051282</v>
+        <v>0.01260504201680672</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>80</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D11">
-        <v>0.006172839506172839</v>
+        <v>0.008620689655172414</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D12">
-        <v>0.005649717514124294</v>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>0.03688524590163934</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>0.03508771929824561</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>0.02702702702702703</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>0.02521008403361345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>0.01977401129943503</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>0.007058823529411765</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>0.004761904761904762</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>0.8105263157894737</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>0.1129568106312292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>0.05102040816326531</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>0.04769001490312966</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>0.02222222222222222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>0.02197802197802198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>0.02112676056338028</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>0.01975308641975309</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>0.01864406779661017</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>0.01574803149606299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>0.01260504201680672</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>82</v>
+        <v>169</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>183</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D13">
-        <v>0.002906976744186046</v>
+        <v>0.005917159763313609</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>0.004651162790697674</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3248,14 +3710,16 @@
     <hyperlink ref="A11" r:id="rId10"/>
     <hyperlink ref="A12" r:id="rId11"/>
     <hyperlink ref="A13" r:id="rId12"/>
+    <hyperlink ref="A14" r:id="rId13"/>
+    <hyperlink ref="A15" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3277,240 +3741,254 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>95</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>204</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D2">
-        <v>0.05990783410138249</v>
+        <v>0.05741626794258373</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>96</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>205</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>0.04424778761061947</v>
+        <v>0.05422314911366007</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>97</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>206</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>0.0396039603960396</v>
+        <v>0.04659498207885305</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>98</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>207</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>0.03703703703703703</v>
+        <v>0.04069767441860465</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>99</v>
+        <v>190</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>208</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>0.03091190108191654</v>
+        <v>0.03271028037383177</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>100</v>
+        <v>191</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>209</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>0.02456140350877193</v>
+        <v>0.03076923076923077</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>101</v>
+        <v>192</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>210</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D8">
-        <v>0.01907356948228883</v>
+        <v>0.02920443101711984</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>102</v>
+        <v>193</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>211</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D9">
-        <v>0.01718213058419244</v>
+        <v>0.02836879432624113</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>103</v>
+        <v>194</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>212</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D10">
-        <v>0.01526717557251908</v>
+        <v>0.02824267782426778</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>104</v>
+        <v>195</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>213</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D11">
-        <v>0.01456310679611651</v>
+        <v>0.02639751552795031</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>105</v>
+        <v>196</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>214</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D12">
-        <v>0.01232032854209446</v>
+        <v>0.02185792349726776</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>106</v>
+        <v>197</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>215</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D13">
-        <v>0.01043478260869565</v>
+        <v>0.02180685358255452</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>107</v>
+        <v>198</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>216</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D14">
-        <v>0.009950248756218905</v>
+        <v>0.02153846153846154</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>108</v>
+        <v>199</v>
       </c>
       <c r="B15" t="s">
-        <v>125</v>
+        <v>217</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D15">
-        <v>0.007194244604316547</v>
+        <v>0.01341281669150522</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>109</v>
+        <v>200</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>218</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D16">
-        <v>0.003703703703703704</v>
+        <v>0.01020082881734141</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>110</v>
+        <v>201</v>
       </c>
       <c r="B17" t="s">
-        <v>127</v>
+        <v>219</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D17">
-        <v>0.002577319587628866</v>
+        <v>0.009036144578313253</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>111</v>
+        <v>202</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>220</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>0.006345177664974619</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19">
+        <v>0.003891050583657588</v>
       </c>
     </row>
   </sheetData>
@@ -3532,439 +4010,7 @@
     <hyperlink ref="A16" r:id="rId15"/>
     <hyperlink ref="A17" r:id="rId16"/>
     <hyperlink ref="A18" r:id="rId17"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>0.08279569892473118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>0.04878048780487805</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>0.03485576923076923</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>0.03485576923076923</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>0.02994011976047904</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>0.02824858757062147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8">
-        <v>0.02586206896551724</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B9" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9">
-        <v>0.01532567049808429</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B10" t="s">
-        <v>147</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>0.01260504201680672</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B11" t="s">
-        <v>148</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11">
-        <v>0.008620689655172414</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B12" t="s">
-        <v>149</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
-    <hyperlink ref="A12" r:id="rId11"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>0.8105263157894737</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>0.1129568106312292</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>0.05102040816326531</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>0.04769001490312966</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B6" t="s">
-        <v>168</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>0.02222222222222222</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>0.02197802197802198</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B8" t="s">
-        <v>170</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8">
-        <v>0.02112676056338028</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B9" t="s">
-        <v>171</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9">
-        <v>0.01975308641975309</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>0.01864406779661017</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B11" t="s">
-        <v>173</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11">
-        <v>0.01574803149606299</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>0.01260504201680672</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B13" t="s">
-        <v>175</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13">
-        <v>0.005917159763313609</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B14" t="s">
-        <v>176</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14">
-        <v>0.004651162790697674</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B15" t="s">
-        <v>177</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
-    <hyperlink ref="A12" r:id="rId11"/>
-    <hyperlink ref="A13" r:id="rId12"/>
-    <hyperlink ref="A14" r:id="rId13"/>
-    <hyperlink ref="A15" r:id="rId14"/>
+    <hyperlink ref="A19" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>